<commit_message>
Added storms summary table to Manuscript
</commit_message>
<xml_diff>
--- a/Data/S storm table summary.xlsx
+++ b/Data/S storm table summary.xlsx
@@ -491,37 +491,37 @@
         <v>8.7</v>
       </c>
       <c r="D2" t="n">
-        <v>1227.304</v>
+        <v>1062.458</v>
       </c>
       <c r="E2" t="n">
-        <v>461234700.0</v>
+        <v>430065000.0</v>
       </c>
       <c r="F2" t="n">
-        <v>1095683.4</v>
+        <v>946938.6000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>634448.7000000001</v>
+        <v>516873.6</v>
       </c>
       <c r="H2" t="n">
-        <v>131.05499999999998</v>
+        <v>125.61599999999999</v>
       </c>
       <c r="I2" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" t="n">
-        <v>152.08999999999997</v>
+        <v>146.17199999999997</v>
       </c>
       <c r="K2" t="n">
-        <v>21.036</v>
+        <v>20.555</v>
       </c>
       <c r="L2" t="n">
-        <v>704.9430000000001</v>
+        <v>574.304</v>
       </c>
       <c r="M2" t="n">
-        <v>524130.34090909094</v>
+        <v>488710.22727272724</v>
       </c>
       <c r="N2" t="n">
-        <v>615.5524719101123</v>
+        <v>531.9879775280899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>